<commit_message>
Update calc height total
</commit_message>
<xml_diff>
--- a/worker-service/templates/template-merge.xlsx
+++ b/worker-service/templates/template-merge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceBuild\github\excel-worker\worker-service\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A5B898-DD23-4E92-9887-3910BAD50CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6B8C4E-A9CA-46E0-92B1-A0A90B069B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26385" yWindow="3060" windowWidth="21555" windowHeight="11745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28440" yWindow="465" windowWidth="20700" windowHeight="13335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -9413,7 +9413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -9439,15 +9439,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -9460,6 +9451,16 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9802,7 +9803,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9825,49 +9826,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
@@ -9906,188 +9907,178 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16" t="s">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16" t="s">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16" t="s">
+      <c r="I6" s="13"/>
+      <c r="J6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16" t="s">
+      <c r="K6" s="13"/>
+      <c r="L6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16" t="s">
+      <c r="M6" s="13"/>
+      <c r="N6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="16"/>
+      <c r="O6" s="13"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16" t="s">
+      <c r="G7" s="13"/>
+      <c r="H7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16" t="s">
+      <c r="I7" s="13"/>
+      <c r="J7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16" t="s">
+      <c r="K7" s="13"/>
+      <c r="L7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16" t="s">
+      <c r="M7" s="13"/>
+      <c r="N7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="16"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16" t="s">
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16" t="s">
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16" t="s">
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16" t="s">
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="13" t="s">
         <v>3024</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:O10"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A12:O12"/>
+  <mergeCells count="27">
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="A6:A10"/>
@@ -10104,9 +10095,17 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D10:O10"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="B6:C7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="D9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Update queue with redis
</commit_message>
<xml_diff>
--- a/worker-service/templates/template-merge.xlsx
+++ b/worker-service/templates/template-merge.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceBuild\github\excel-worker\worker-service\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A5B898-DD23-4E92-9887-3910BAD50CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635524D3-CB74-42BA-9BD2-E8248AFCFF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26385" yWindow="3060" windowWidth="21555" windowHeight="11745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28155" yWindow="1665" windowWidth="20700" windowHeight="13335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="config" sheetId="2" r:id="rId2"/>
-    <sheet name="data" sheetId="3" r:id="rId3"/>
+    <sheet name="Report-template" sheetId="4" r:id="rId2"/>
+    <sheet name="config" sheetId="2" r:id="rId3"/>
+    <sheet name="data" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -172,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3056" uniqueCount="3026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3073" uniqueCount="3026">
   <si>
     <t>begin</t>
   </si>
@@ -9439,15 +9440,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -9458,6 +9450,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -9799,10 +9800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9825,49 +9826,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
@@ -9905,208 +9906,51 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="O6" s="16"/>
-    </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" s="16"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
+      <c r="A7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
-        <v>3024</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:O10"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="A12:O12"/>
+  <mergeCells count="5">
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="G8:I8"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="A9:O9"/>
+    <mergeCell ref="A7:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -10114,6 +9958,322 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C692AC29-7237-4D54-BB1B-FABBC6A90BE0}">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="10" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.75" customWidth="1"/>
+    <col min="6" max="6" width="10.75" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="8" max="8" width="10.75" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.75" customWidth="1"/>
+    <col min="10" max="10" width="10.75" style="5" customWidth="1"/>
+    <col min="11" max="11" width="10.75" customWidth="1"/>
+    <col min="12" max="12" width="10.75" style="5" customWidth="1"/>
+    <col min="13" max="13" width="10.75" customWidth="1"/>
+    <col min="14" max="14" width="10.75" style="5" customWidth="1"/>
+    <col min="15" max="15" width="10.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="13"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="13"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="13" t="s">
+        <v>3024</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:O10"/>
+    <mergeCell ref="A12:O12"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -10193,7 +10353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D1002"/>
   <sheetViews>

</xml_diff>